<commit_message>
fixed circumferential blade thickness to correctly compute the azimuthal thickness
</commit_message>
<xml_diff>
--- a/XPROP_validation/XPROP-TUD-Geometry.xlsx
+++ b/XPROP_validation/XPROP-TUD-Geometry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b266c95a83fbf4bb/Documenten/TU Delft Aerospace Engineering/Msc2/AE5222 - Thesis/Software/Conceptual-Investigation-of-Alternative-Electric-Ducted-Fan-Architectures/XPROP_validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_043F22CD0A92D18E0D018920400120A071568E56" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A1FFE33-C69A-452D-B259-315809BDC437}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="11_043F22CD0A92D18E0D018920400120A071568E56" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7A55389-EC36-4751-AE55-A08B636C4AB7}"/>
   <bookViews>
-    <workbookView xWindow="11442" yWindow="0" windowWidth="11676" windowHeight="13758" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="XPROP Geometry" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="90">
   <si>
     <t>Station W</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -362,14 +362,18 @@
   <si>
     <t>c/D</t>
   </si>
+  <si>
+    <t>-</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.000000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -430,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -460,6 +464,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,6 +480,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -802,72 +811,72 @@
   </sheetPr>
   <dimension ref="A1:AA323"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.47265625" customWidth="1"/>
-    <col min="13" max="13" width="13.76171875" customWidth="1"/>
+    <col min="12" max="12" width="13.4609375" customWidth="1"/>
+    <col min="13" max="13" width="13.765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>71</v>
       </c>
       <c r="L7" s="14"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="L11" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>70</v>
       </c>
@@ -879,10 +888,14 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>79.128</v>
       </c>
+      <c r="C13">
+        <f>A13/1000</f>
+        <v>7.9128000000000004E-2</v>
+      </c>
       <c r="G13" s="5">
         <v>203.2</v>
       </c>
@@ -890,13 +903,13 @@
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G14" s="5"/>
       <c r="L14" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>58</v>
       </c>
@@ -904,12 +917,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="L16" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>68</v>
       </c>
@@ -947,10 +960,12 @@
         <v>88</v>
       </c>
       <c r="Q17" s="9"/>
-      <c r="R17" s="13"/>
+      <c r="R17" s="13" t="s">
+        <v>89</v>
+      </c>
       <c r="S17" s="9"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
@@ -991,11 +1006,17 @@
         <v>8.0152805118110237E-2</v>
       </c>
       <c r="Q18" s="12"/>
-      <c r="R18" s="11"/>
+      <c r="R18" s="11">
+        <f>L18/K18</f>
+        <v>0.40167802026763594</v>
+      </c>
       <c r="S18" s="5"/>
-      <c r="T18" s="5"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T18" s="15">
+        <f>I18/1000</f>
+        <v>3.2511999999999999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1036,11 +1057,17 @@
         <v>7.8986220472440957E-2</v>
       </c>
       <c r="Q19" s="12"/>
-      <c r="R19" s="11"/>
+      <c r="R19" s="11">
+        <f t="shared" ref="R19:R42" si="3">L19/K19</f>
+        <v>0.40138940809968848</v>
+      </c>
       <c r="S19" s="5"/>
-      <c r="T19" s="5"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T19" s="15">
+        <f t="shared" ref="T19:T42" si="4">I19/1000</f>
+        <v>3.9623999999999999E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>3</v>
       </c>
@@ -1081,11 +1108,17 @@
         <v>7.7820127952755919E-2</v>
       </c>
       <c r="Q20" s="12"/>
-      <c r="R20" s="11"/>
+      <c r="R20" s="11">
+        <f t="shared" si="3"/>
+        <v>0.40104533913444906</v>
+      </c>
       <c r="S20" s="5"/>
-      <c r="T20" s="5"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T20" s="15">
+        <f t="shared" si="4"/>
+        <v>4.6736E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>4</v>
       </c>
@@ -1126,11 +1159,17 @@
         <v>7.665009842519685E-2</v>
       </c>
       <c r="Q21" s="12"/>
-      <c r="R21" s="11"/>
+      <c r="R21" s="11">
+        <f t="shared" si="3"/>
+        <v>0.40182853620797032</v>
+      </c>
       <c r="S21" s="5"/>
-      <c r="T21" s="5"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T21" s="15">
+        <f t="shared" si="4"/>
+        <v>5.3848E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>5</v>
       </c>
@@ -1171,11 +1210,17 @@
         <v>7.5486220472440954E-2</v>
       </c>
       <c r="Q22" s="12"/>
-      <c r="R22" s="11"/>
+      <c r="R22" s="11">
+        <f t="shared" si="3"/>
+        <v>0.40856194747959418</v>
+      </c>
       <c r="S22" s="5"/>
-      <c r="T22" s="5"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T22" s="15">
+        <f t="shared" si="4"/>
+        <v>6.0959999999999993E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>6</v>
       </c>
@@ -1216,11 +1261,17 @@
         <v>7.4387549212598436E-2</v>
       </c>
       <c r="Q23" s="12"/>
-      <c r="R23" s="11"/>
+      <c r="R23" s="11">
+        <f t="shared" si="3"/>
+        <v>0.41339547684338313</v>
+      </c>
       <c r="S23" s="5"/>
-      <c r="T23" s="5"/>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T23" s="15">
+        <f t="shared" si="4"/>
+        <v>6.8072000000000008E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>7</v>
       </c>
@@ -1261,11 +1312,17 @@
         <v>7.3456938976377964E-2</v>
       </c>
       <c r="Q24" s="12"/>
-      <c r="R24" s="11"/>
+      <c r="R24" s="11">
+        <f t="shared" si="3"/>
+        <v>0.41656589477069228</v>
+      </c>
       <c r="S24" s="5"/>
-      <c r="T24" s="5"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T24" s="15">
+        <f t="shared" si="4"/>
+        <v>7.5184000000000001E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>8</v>
       </c>
@@ -1306,11 +1363,17 @@
         <v>7.2795029527559063E-2</v>
       </c>
       <c r="Q25" s="12"/>
-      <c r="R25" s="11"/>
+      <c r="R25" s="11">
+        <f t="shared" si="3"/>
+        <v>0.41855198266624755</v>
+      </c>
       <c r="S25" s="5"/>
-      <c r="T25" s="5"/>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T25" s="15">
+        <f t="shared" si="4"/>
+        <v>8.2296000000000008E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>9</v>
       </c>
@@ -1351,11 +1414,17 @@
         <v>7.2553395669291351E-2</v>
       </c>
       <c r="Q26" s="12"/>
-      <c r="R26" s="11"/>
+      <c r="R26" s="11">
+        <f t="shared" si="3"/>
+        <v>0.42012568804539152</v>
+      </c>
       <c r="S26" s="5"/>
-      <c r="T26" s="5"/>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T26" s="15">
+        <f t="shared" si="4"/>
+        <v>8.9408000000000001E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>10</v>
       </c>
@@ -1396,11 +1465,17 @@
         <v>7.2788139763779527E-2</v>
       </c>
       <c r="Q27" s="12"/>
-      <c r="R27" s="11"/>
+      <c r="R27" s="11">
+        <f t="shared" si="3"/>
+        <v>0.42140758795311872</v>
+      </c>
       <c r="S27" s="5"/>
-      <c r="T27" s="5"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T27" s="15">
+        <f t="shared" si="4"/>
+        <v>9.6519999999999995E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>11</v>
       </c>
@@ -1441,11 +1516,17 @@
         <v>7.3420029527559064E-2</v>
       </c>
       <c r="Q28" s="12"/>
-      <c r="R28" s="11"/>
+      <c r="R28" s="11">
+        <f t="shared" si="3"/>
+        <v>0.42241913807607107</v>
+      </c>
       <c r="S28" s="5"/>
-      <c r="T28" s="5"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T28" s="15">
+        <f t="shared" si="4"/>
+        <v>0.10363199999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>12</v>
       </c>
@@ -1486,11 +1567,17 @@
         <v>7.4251968503937005E-2</v>
       </c>
       <c r="Q29" s="12"/>
-      <c r="R29" s="11"/>
+      <c r="R29" s="11">
+        <f t="shared" si="3"/>
+        <v>0.4235220042417816</v>
+      </c>
       <c r="S29" s="5"/>
-      <c r="T29" s="5"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T29" s="15">
+        <f t="shared" si="4"/>
+        <v>0.110744</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>13</v>
       </c>
@@ -1531,11 +1618,17 @@
         <v>7.5086122047244103E-2</v>
       </c>
       <c r="Q30" s="12"/>
-      <c r="R30" s="11"/>
+      <c r="R30" s="11">
+        <f t="shared" si="3"/>
+        <v>0.42372931345240045</v>
+      </c>
       <c r="S30" s="5"/>
-      <c r="T30" s="5"/>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T30" s="15">
+        <f t="shared" si="4"/>
+        <v>0.11785599999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>14</v>
       </c>
@@ -1576,11 +1669,17 @@
         <v>7.5726377952755913E-2</v>
       </c>
       <c r="Q31" s="12"/>
-      <c r="R31" s="11"/>
+      <c r="R31" s="11">
+        <f t="shared" si="3"/>
+        <v>0.42424094725623229</v>
+      </c>
       <c r="S31" s="5"/>
-      <c r="T31" s="5"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T31" s="15">
+        <f t="shared" si="4"/>
+        <v>0.124968</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>15</v>
       </c>
@@ -1621,11 +1720,17 @@
         <v>7.6125000000000012E-2</v>
       </c>
       <c r="Q32" s="12"/>
-      <c r="R32" s="11"/>
+      <c r="R32" s="11">
+        <f t="shared" si="3"/>
+        <v>0.42489300906352223</v>
+      </c>
       <c r="S32" s="5"/>
-      <c r="T32" s="5"/>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T32" s="15">
+        <f t="shared" si="4"/>
+        <v>0.13207999999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>16</v>
       </c>
@@ -1666,11 +1771,17 @@
         <v>7.6408218503937003E-2</v>
       </c>
       <c r="Q33" s="12"/>
-      <c r="R33" s="11"/>
+      <c r="R33" s="11">
+        <f t="shared" si="3"/>
+        <v>0.4256270872044905</v>
+      </c>
       <c r="S33" s="5"/>
-      <c r="T33" s="5"/>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T33" s="15">
+        <f t="shared" si="4"/>
+        <v>0.13919200000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>17</v>
       </c>
@@ -1711,11 +1822,17 @@
         <v>7.6687500000000006E-2</v>
       </c>
       <c r="Q34" s="12"/>
-      <c r="R34" s="11"/>
+      <c r="R34" s="11">
+        <f t="shared" si="3"/>
+        <v>0.42641613563585723</v>
+      </c>
       <c r="S34" s="5"/>
-      <c r="T34" s="5"/>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T34" s="15">
+        <f t="shared" si="4"/>
+        <v>0.14630399999999996</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>18</v>
       </c>
@@ -1756,11 +1873,17 @@
         <v>7.6672982283464572E-2</v>
       </c>
       <c r="Q35" s="12"/>
-      <c r="R35" s="11"/>
+      <c r="R35" s="11">
+        <f t="shared" si="3"/>
+        <v>0.42731523528637766</v>
+      </c>
       <c r="S35" s="5"/>
-      <c r="T35" s="5"/>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T35" s="15">
+        <f t="shared" si="4"/>
+        <v>0.153416</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>19</v>
       </c>
@@ -1801,11 +1924,17 @@
         <v>7.5735482283464578E-2</v>
       </c>
       <c r="Q36" s="12"/>
-      <c r="R36" s="11"/>
+      <c r="R36" s="11">
+        <f t="shared" si="3"/>
+        <v>0.42826091900620228</v>
+      </c>
       <c r="S36" s="5"/>
-      <c r="T36" s="5"/>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T36" s="15">
+        <f t="shared" si="4"/>
+        <v>0.160528</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>20</v>
       </c>
@@ -1846,11 +1975,17 @@
         <v>7.3267962598425204E-2</v>
       </c>
       <c r="Q37" s="12"/>
-      <c r="R37" s="11"/>
+      <c r="R37" s="11">
+        <f t="shared" si="3"/>
+        <v>0.42918313681106662</v>
+      </c>
       <c r="S37" s="5"/>
-      <c r="T37" s="5"/>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T37" s="15">
+        <f t="shared" si="4"/>
+        <v>0.16763999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>21</v>
       </c>
@@ -1891,11 +2026,17 @@
         <v>6.8986220472440948E-2</v>
       </c>
       <c r="Q38" s="12"/>
-      <c r="R38" s="11"/>
+      <c r="R38" s="11">
+        <f t="shared" si="3"/>
+        <v>0.43004708232272792</v>
+      </c>
       <c r="S38" s="5"/>
-      <c r="T38" s="5"/>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T38" s="15">
+        <f t="shared" si="4"/>
+        <v>0.17475199999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="G39" s="3" t="s">
         <v>49</v>
       </c>
@@ -1927,10 +2068,17 @@
         <v>6.278912401574803E-2</v>
       </c>
       <c r="Q39" s="12"/>
-      <c r="R39" s="11"/>
+      <c r="R39" s="11">
+        <f t="shared" si="3"/>
+        <v>0.43070441853629871</v>
+      </c>
       <c r="S39" s="5"/>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T39" s="15">
+        <f t="shared" si="4"/>
+        <v>0.181864</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="G40" s="3" t="s">
         <v>50</v>
       </c>
@@ -1962,10 +2110,17 @@
         <v>5.4702017716535434E-2</v>
       </c>
       <c r="Q40" s="12"/>
-      <c r="R40" s="11"/>
+      <c r="R40" s="11">
+        <f t="shared" si="3"/>
+        <v>0.43109815617001568</v>
+      </c>
       <c r="S40" s="5"/>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T40" s="15">
+        <f t="shared" si="4"/>
+        <v>0.18897600000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="G41" s="3" t="s">
         <v>51</v>
       </c>
@@ -1997,10 +2152,17 @@
         <v>4.5604822834645668E-2</v>
       </c>
       <c r="Q41" s="12"/>
-      <c r="R41" s="11"/>
+      <c r="R41" s="11">
+        <f t="shared" si="3"/>
+        <v>0.43097475962835469</v>
+      </c>
       <c r="S41" s="5"/>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T41" s="15">
+        <f t="shared" si="4"/>
+        <v>0.19608799999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="G42" s="3" t="s">
         <v>52</v>
       </c>
@@ -2032,17 +2194,24 @@
         <v>3.4027805118110238E-2</v>
       </c>
       <c r="Q42" s="12"/>
-      <c r="R42" s="11"/>
+      <c r="R42" s="11">
+        <f t="shared" si="3"/>
+        <v>0.4312056635017969</v>
+      </c>
       <c r="S42" s="5"/>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T42" s="15">
+        <f t="shared" si="4"/>
+        <v>0.20319999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="G43" s="3"/>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
       <c r="J43" s="4"/>
       <c r="P43" s="10"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>72</v>
       </c>
@@ -2051,31 +2220,31 @@
       <c r="I44" s="5"/>
       <c r="J44" s="4"/>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="G45" s="3"/>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
       <c r="J45" s="4"/>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A49" s="6"/>
     </row>
-    <row r="50" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>23</v>
       </c>
@@ -2095,7 +2264,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>53</v>
       </c>
@@ -2151,7 +2320,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="8">
         <v>0</v>
       </c>
@@ -2207,7 +2376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="8">
         <v>8.14E-2</v>
       </c>
@@ -2263,7 +2432,7 @@
         <v>-0.2717</v>
       </c>
     </row>
-    <row r="55" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="8">
         <v>0.16289999999999999</v>
       </c>
@@ -2319,7 +2488,7 @@
         <v>-0.37880000000000003</v>
       </c>
     </row>
-    <row r="56" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="8">
         <v>0.24429999999999999</v>
       </c>
@@ -2375,7 +2544,7 @@
         <v>-0.45839999999999997</v>
       </c>
     </row>
-    <row r="57" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="8">
         <v>0.32569999999999999</v>
       </c>
@@ -2431,7 +2600,7 @@
         <v>-0.52370000000000005</v>
       </c>
     </row>
-    <row r="58" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="8">
         <v>0.40720000000000001</v>
       </c>
@@ -2487,7 +2656,7 @@
         <v>-0.57979999999999998</v>
       </c>
     </row>
-    <row r="59" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="8">
         <v>0.48859999999999998</v>
       </c>
@@ -2543,7 +2712,7 @@
         <v>-0.62929999999999997</v>
       </c>
     </row>
-    <row r="60" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="8">
         <v>0.56999999999999995</v>
       </c>
@@ -2599,7 +2768,7 @@
         <v>-0.67379999999999995</v>
       </c>
     </row>
-    <row r="61" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="8">
         <v>0.65149999999999997</v>
       </c>
@@ -2655,7 +2824,7 @@
         <v>-0.71430000000000005</v>
       </c>
     </row>
-    <row r="62" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="8">
         <v>0.81440000000000001</v>
       </c>
@@ -2711,7 +2880,7 @@
         <v>-0.78590000000000004</v>
       </c>
     </row>
-    <row r="63" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="8">
         <v>0.97719999999999996</v>
       </c>
@@ -2767,7 +2936,7 @@
         <v>-0.84789999999999999</v>
       </c>
     </row>
-    <row r="64" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="8">
         <v>1.1400999999999999</v>
       </c>
@@ -2823,7 +2992,7 @@
         <v>-0.90259999999999996</v>
       </c>
     </row>
-    <row r="65" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="8">
         <v>1.3029999999999999</v>
       </c>
@@ -2879,7 +3048,7 @@
         <v>-0.95140000000000002</v>
       </c>
     </row>
-    <row r="66" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="8">
         <v>1.4658</v>
       </c>
@@ -2935,7 +3104,7 @@
         <v>-0.99529999999999996</v>
       </c>
     </row>
-    <row r="67" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="8">
         <v>1.6287</v>
       </c>
@@ -2991,7 +3160,7 @@
         <v>-1.0350999999999999</v>
       </c>
     </row>
-    <row r="68" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="8">
         <v>1.9543999999999999</v>
       </c>
@@ -3047,7 +3216,7 @@
         <v>-1.1046</v>
       </c>
     </row>
-    <row r="69" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="8">
         <v>2.2801999999999998</v>
       </c>
@@ -3103,7 +3272,7 @@
         <v>-1.163</v>
       </c>
     </row>
-    <row r="70" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="8">
         <v>2.6059000000000001</v>
       </c>
@@ -3159,7 +3328,7 @@
         <v>-1.2126999999999999</v>
       </c>
     </row>
-    <row r="71" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="8">
         <v>2.9317000000000002</v>
       </c>
@@ -3215,7 +3384,7 @@
         <v>-1.2549999999999999</v>
       </c>
     </row>
-    <row r="72" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="8">
         <v>3.2574000000000001</v>
       </c>
@@ -3271,7 +3440,7 @@
         <v>-1.2911999999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="8">
         <v>3.9089</v>
       </c>
@@ -3327,7 +3496,7 @@
         <v>-1.3482000000000001</v>
       </c>
     </row>
-    <row r="74" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="8">
         <v>4.5603999999999996</v>
       </c>
@@ -3383,7 +3552,7 @@
         <v>-1.3886000000000001</v>
       </c>
     </row>
-    <row r="75" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="8">
         <v>5.2119</v>
       </c>
@@ -3439,7 +3608,7 @@
         <v>-1.4157999999999999</v>
       </c>
     </row>
-    <row r="76" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="8">
         <v>5.8632999999999997</v>
       </c>
@@ -3495,7 +3664,7 @@
         <v>-1.4319999999999999</v>
       </c>
     </row>
-    <row r="77" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="8">
         <v>6.5148000000000001</v>
       </c>
@@ -3551,7 +3720,7 @@
         <v>-1.4391</v>
       </c>
     </row>
-    <row r="78" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="8">
         <v>7.8178000000000001</v>
       </c>
@@ -3607,7 +3776,7 @@
         <v>-1.4309000000000001</v>
       </c>
     </row>
-    <row r="79" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="8">
         <v>8.1434999999999995</v>
       </c>
@@ -3664,7 +3833,7 @@
         <v>-1.425</v>
       </c>
     </row>
-    <row r="80" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="8">
         <v>9.1206999999999994</v>
       </c>
@@ -3720,7 +3889,7 @@
         <v>-1.4036</v>
       </c>
     </row>
-    <row r="81" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="8">
         <v>10.4237</v>
       </c>
@@ -3776,7 +3945,7 @@
         <v>-1.3621000000000001</v>
       </c>
     </row>
-    <row r="82" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="8">
         <v>11.726699999999999</v>
       </c>
@@ -3832,7 +4001,7 @@
         <v>-1.3095000000000001</v>
       </c>
     </row>
-    <row r="83" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="8">
         <v>13.0296</v>
       </c>
@@ -3888,7 +4057,7 @@
         <v>-1.2491000000000001</v>
       </c>
     </row>
-    <row r="84" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="8">
         <v>14.332599999999999</v>
       </c>
@@ -3944,7 +4113,7 @@
         <v>-1.1831</v>
       </c>
     </row>
-    <row r="85" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="8">
         <v>15.6356</v>
       </c>
@@ -4000,7 +4169,7 @@
         <v>-1.1134999999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="8">
         <v>16.938500000000001</v>
       </c>
@@ -4056,7 +4225,7 @@
         <v>-1.0416000000000001</v>
       </c>
     </row>
-    <row r="87" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="8">
         <v>18.241499999999998</v>
       </c>
@@ -4112,7 +4281,7 @@
         <v>-0.96860000000000002</v>
       </c>
     </row>
-    <row r="88" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="8">
         <v>19.544499999999999</v>
       </c>
@@ -4168,7 +4337,7 @@
         <v>-0.89529999999999998</v>
       </c>
     </row>
-    <row r="89" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="8">
         <v>20.8474</v>
       </c>
@@ -4224,7 +4393,7 @@
         <v>-0.82240000000000002</v>
       </c>
     </row>
-    <row r="90" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="8">
         <v>22.150400000000001</v>
       </c>
@@ -4280,7 +4449,7 @@
         <v>-0.74390000000000001</v>
       </c>
     </row>
-    <row r="91" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="8">
         <v>23.453399999999998</v>
       </c>
@@ -4336,7 +4505,7 @@
         <v>-0.66449999999999998</v>
       </c>
     </row>
-    <row r="92" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="8">
         <v>24.7563</v>
       </c>
@@ -4392,7 +4561,7 @@
         <v>-0.5867</v>
       </c>
     </row>
-    <row r="93" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="8">
         <v>26.0593</v>
       </c>
@@ -4448,7 +4617,7 @@
         <v>-0.5111</v>
       </c>
     </row>
-    <row r="94" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="8">
         <v>27.362200000000001</v>
       </c>
@@ -4504,7 +4673,7 @@
         <v>-0.43819999999999998</v>
       </c>
     </row>
-    <row r="95" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="8">
         <v>28.665199999999999</v>
       </c>
@@ -4560,7 +4729,7 @@
         <v>-0.36909999999999998</v>
       </c>
     </row>
-    <row r="96" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="8">
         <v>29.9682</v>
       </c>
@@ -4616,7 +4785,7 @@
         <v>-0.30599999999999999</v>
       </c>
     </row>
-    <row r="97" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="8">
         <v>31.271100000000001</v>
       </c>
@@ -4672,7 +4841,7 @@
         <v>-0.25319999999999998</v>
       </c>
     </row>
-    <row r="98" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="8">
         <v>31.922599999999999</v>
       </c>
@@ -4728,7 +4897,7 @@
         <v>-0.2339</v>
       </c>
     </row>
-    <row r="99" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="8">
         <v>32.574100000000001</v>
       </c>
@@ -4784,7 +4953,7 @@
         <v>-0.2253</v>
       </c>
     </row>
-    <row r="103" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>17</v>
       </c>
@@ -4804,7 +4973,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="105" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>53</v>
       </c>
@@ -4860,7 +5029,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="106" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A106" s="8">
         <v>0</v>
       </c>
@@ -4916,7 +5085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A107" s="8">
         <v>7.46E-2</v>
       </c>
@@ -4972,7 +5141,7 @@
         <v>-0.17580000000000001</v>
       </c>
     </row>
-    <row r="108" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" s="8">
         <v>0.14929999999999999</v>
       </c>
@@ -5028,7 +5197,7 @@
         <v>-0.24</v>
       </c>
     </row>
-    <row r="109" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" s="8">
         <v>0.22389999999999999</v>
       </c>
@@ -5084,7 +5253,7 @@
         <v>-0.28549999999999998</v>
       </c>
     </row>
-    <row r="110" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A110" s="8">
         <v>0.29849999999999999</v>
       </c>
@@ -5140,7 +5309,7 @@
         <v>-0.3211</v>
       </c>
     </row>
-    <row r="111" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A111" s="8">
         <v>0.37319999999999998</v>
       </c>
@@ -5196,7 +5365,7 @@
         <v>-0.35039999999999999</v>
       </c>
     </row>
-    <row r="112" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112" s="8">
         <v>0.44779999999999998</v>
       </c>
@@ -5252,7 +5421,7 @@
         <v>-0.37509999999999999</v>
       </c>
     </row>
-    <row r="113" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A113" s="8">
         <v>0.52239999999999998</v>
       </c>
@@ -5308,7 +5477,7 @@
         <v>-0.39629999999999999</v>
       </c>
     </row>
-    <row r="114" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A114" s="8">
         <v>0.59709999999999996</v>
       </c>
@@ -5364,7 +5533,7 @@
         <v>-0.41470000000000001</v>
       </c>
     </row>
-    <row r="115" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A115" s="8">
         <v>0.74629999999999996</v>
       </c>
@@ -5420,7 +5589,7 @@
         <v>-0.44490000000000002</v>
       </c>
     </row>
-    <row r="116" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A116" s="8">
         <v>0.89559999999999995</v>
       </c>
@@ -5476,7 +5645,7 @@
         <v>-0.46829999999999999</v>
       </c>
     </row>
-    <row r="117" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A117" s="8">
         <v>1.0448999999999999</v>
       </c>
@@ -5532,7 +5701,7 @@
         <v>-0.48670000000000002</v>
       </c>
     </row>
-    <row r="118" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A118" s="8">
         <v>1.1940999999999999</v>
       </c>
@@ -5588,7 +5757,7 @@
         <v>-0.50090000000000001</v>
       </c>
     </row>
-    <row r="119" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A119" s="8">
         <v>1.3433999999999999</v>
       </c>
@@ -5644,7 +5813,7 @@
         <v>-0.51180000000000003</v>
       </c>
     </row>
-    <row r="120" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A120" s="8">
         <v>1.4925999999999999</v>
       </c>
@@ -5700,7 +5869,7 @@
         <v>-0.51990000000000003</v>
       </c>
     </row>
-    <row r="121" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A121" s="8">
         <v>1.7911999999999999</v>
       </c>
@@ -5756,7 +5925,7 @@
         <v>-0.52929999999999999</v>
       </c>
     </row>
-    <row r="122" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A122" s="8">
         <v>2.0897000000000001</v>
       </c>
@@ -5812,7 +5981,7 @@
         <v>-0.53159999999999996</v>
       </c>
     </row>
-    <row r="123" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A123" s="8">
         <v>2.3881999999999999</v>
       </c>
@@ -5868,7 +6037,7 @@
         <v>-0.52839999999999998</v>
       </c>
     </row>
-    <row r="124" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A124" s="8">
         <v>2.6867999999999999</v>
       </c>
@@ -5924,7 +6093,7 @@
         <v>-0.52100000000000002</v>
       </c>
     </row>
-    <row r="125" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A125" s="8">
         <v>2.9853000000000001</v>
       </c>
@@ -5980,7 +6149,7 @@
         <v>-0.51019999999999999</v>
       </c>
     </row>
-    <row r="126" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A126" s="8">
         <v>3.5823</v>
       </c>
@@ -6036,7 +6205,7 @@
         <v>-0.48149999999999998</v>
       </c>
     </row>
-    <row r="127" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A127" s="8">
         <v>4.1794000000000002</v>
       </c>
@@ -6092,7 +6261,7 @@
         <v>-0.44669999999999999</v>
       </c>
     </row>
-    <row r="128" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A128" s="8">
         <v>4.7765000000000004</v>
       </c>
@@ -6148,7 +6317,7 @@
         <v>-0.4088</v>
       </c>
     </row>
-    <row r="129" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A129" s="8">
         <v>5.3734999999999999</v>
       </c>
@@ -6204,7 +6373,7 @@
         <v>-0.37030000000000002</v>
       </c>
     </row>
-    <row r="130" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A130" s="8">
         <v>5.9706000000000001</v>
       </c>
@@ -6260,7 +6429,7 @@
         <v>-0.33310000000000001</v>
       </c>
     </row>
-    <row r="131" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A131" s="8">
         <v>7.1646999999999998</v>
       </c>
@@ -6316,7 +6485,7 @@
         <v>-0.26860000000000001</v>
       </c>
     </row>
-    <row r="132" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A132" s="8">
         <v>7.4631999999999996</v>
       </c>
@@ -6372,7 +6541,7 @@
         <v>-0.25540000000000002</v>
       </c>
     </row>
-    <row r="133" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A133" s="8">
         <v>8.3588000000000005</v>
       </c>
@@ -6428,7 +6597,7 @@
         <v>-0.2235</v>
       </c>
     </row>
-    <row r="134" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A134" s="8">
         <v>9.5528999999999993</v>
       </c>
@@ -6484,7 +6653,7 @@
         <v>-0.1842</v>
       </c>
     </row>
-    <row r="135" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A135" s="8">
         <v>10.747</v>
       </c>
@@ -6540,7 +6709,7 @@
         <v>-0.14990000000000001</v>
       </c>
     </row>
-    <row r="136" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A136" s="8">
         <v>11.9412</v>
       </c>
@@ -6596,7 +6765,7 @@
         <v>-0.1216</v>
       </c>
     </row>
-    <row r="137" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A137" s="8">
         <v>13.135300000000001</v>
       </c>
@@ -6652,7 +6821,7 @@
         <v>-9.98E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A138" s="8">
         <v>14.3294</v>
       </c>
@@ -6708,7 +6877,7 @@
         <v>-8.4699999999999998E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A139" s="8">
         <v>15.5235</v>
       </c>
@@ -6764,7 +6933,7 @@
         <v>-7.6200000000000004E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A140" s="8">
         <v>16.717600000000001</v>
       </c>
@@ -6820,7 +6989,7 @@
         <v>-7.3899999999999993E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A141" s="8">
         <v>17.9117</v>
       </c>
@@ -6876,7 +7045,7 @@
         <v>-7.7299999999999994E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A142" s="8">
         <v>19.105899999999998</v>
       </c>
@@ -6932,7 +7101,7 @@
         <v>-8.5599999999999996E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A143" s="8">
         <v>20.3</v>
       </c>
@@ -6988,7 +7157,7 @@
         <v>-9.1399999999999995E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A144" s="8">
         <v>21.4941</v>
       </c>
@@ -7044,7 +7213,7 @@
         <v>-9.7900000000000001E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A145" s="8">
         <v>22.688199999999998</v>
       </c>
@@ -7100,7 +7269,7 @@
         <v>-0.1061</v>
       </c>
     </row>
-    <row r="146" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A146" s="8">
         <v>23.882300000000001</v>
       </c>
@@ -7156,7 +7325,7 @@
         <v>-0.1149</v>
       </c>
     </row>
-    <row r="147" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A147" s="8">
         <v>25.0764</v>
       </c>
@@ -7212,7 +7381,7 @@
         <v>-0.1231</v>
       </c>
     </row>
-    <row r="148" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A148" s="8">
         <v>26.270600000000002</v>
       </c>
@@ -7268,7 +7437,7 @@
         <v>-0.1298</v>
       </c>
     </row>
-    <row r="149" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A149" s="8">
         <v>27.464700000000001</v>
       </c>
@@ -7324,7 +7493,7 @@
         <v>-0.1346</v>
       </c>
     </row>
-    <row r="150" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A150" s="8">
         <v>28.658799999999999</v>
       </c>
@@ -7380,7 +7549,7 @@
         <v>-0.1386</v>
       </c>
     </row>
-    <row r="151" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A151" s="8">
         <v>29.255800000000001</v>
       </c>
@@ -7436,7 +7605,7 @@
         <v>-0.1419</v>
       </c>
     </row>
-    <row r="152" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A152" s="8">
         <v>29.852900000000002</v>
       </c>
@@ -7492,7 +7661,7 @@
         <v>-0.14960000000000001</v>
       </c>
     </row>
-    <row r="156" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="156" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>10</v>
       </c>
@@ -7512,7 +7681,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="158" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="158" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>53</v>
       </c>
@@ -7568,7 +7737,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="159" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="159" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A159" s="8">
         <v>0</v>
       </c>
@@ -7624,7 +7793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A160" s="8">
         <v>7.6300000000000007E-2</v>
       </c>
@@ -7680,7 +7849,7 @@
         <v>-0.1646</v>
       </c>
     </row>
-    <row r="161" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="161" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A161" s="8">
         <v>0.15260000000000001</v>
       </c>
@@ -7736,7 +7905,7 @@
         <v>-0.22109999999999999</v>
       </c>
     </row>
-    <row r="162" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="162" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A162" s="8">
         <v>0.22889999999999999</v>
       </c>
@@ -7792,7 +7961,7 @@
         <v>-0.2591</v>
       </c>
     </row>
-    <row r="163" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="163" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A163" s="8">
         <v>0.30509999999999998</v>
       </c>
@@ -7848,7 +8017,7 @@
         <v>-0.2873</v>
       </c>
     </row>
-    <row r="164" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="164" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A164" s="8">
         <v>0.38140000000000002</v>
       </c>
@@ -7904,7 +8073,7 @@
         <v>-0.30909999999999999</v>
       </c>
     </row>
-    <row r="165" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="165" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A165" s="8">
         <v>0.4577</v>
       </c>
@@ -7960,7 +8129,7 @@
         <v>-0.32619999999999999</v>
       </c>
     </row>
-    <row r="166" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="166" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A166" s="8">
         <v>0.53400000000000003</v>
       </c>
@@ -8016,7 +8185,7 @@
         <v>-0.33979999999999999</v>
       </c>
     </row>
-    <row r="167" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="167" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A167" s="8">
         <v>0.61029999999999995</v>
       </c>
@@ -8072,7 +8241,7 @@
         <v>-0.35049999999999998</v>
       </c>
     </row>
-    <row r="168" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="168" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A168" s="8">
         <v>0.76290000000000002</v>
       </c>
@@ -8128,7 +8297,7 @@
         <v>-0.36520000000000002</v>
       </c>
     </row>
-    <row r="169" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="169" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A169" s="8">
         <v>0.91539999999999999</v>
       </c>
@@ -8185,7 +8354,7 @@
         <v>-0.37290000000000001</v>
       </c>
     </row>
-    <row r="170" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="170" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A170" s="8">
         <v>1.0680000000000001</v>
       </c>
@@ -8241,7 +8410,7 @@
         <v>-0.37509999999999999</v>
       </c>
     </row>
-    <row r="171" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="171" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A171" s="8">
         <v>1.2205999999999999</v>
       </c>
@@ -8297,7 +8466,7 @@
         <v>-0.37319999999999998</v>
       </c>
     </row>
-    <row r="172" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="172" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A172" s="8">
         <v>1.3732</v>
       </c>
@@ -8353,7 +8522,7 @@
         <v>-0.36770000000000003</v>
       </c>
     </row>
-    <row r="173" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="173" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A173" s="8">
         <v>1.5258</v>
       </c>
@@ -8409,7 +8578,7 @@
         <v>-0.35920000000000002</v>
       </c>
     </row>
-    <row r="174" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="174" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A174" s="8">
         <v>1.8309</v>
       </c>
@@ -8465,7 +8634,7 @@
         <v>-0.33529999999999999</v>
       </c>
     </row>
-    <row r="175" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="175" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A175" s="8">
         <v>2.1360000000000001</v>
       </c>
@@ -8521,7 +8690,7 @@
         <v>-0.30420000000000003</v>
       </c>
     </row>
-    <row r="176" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="176" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A176" s="8">
         <v>2.4411999999999998</v>
       </c>
@@ -8577,7 +8746,7 @@
         <v>-0.2676</v>
       </c>
     </row>
-    <row r="177" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="177" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A177" s="8">
         <v>2.7464</v>
       </c>
@@ -8633,7 +8802,7 @@
         <v>-0.2271</v>
       </c>
     </row>
-    <row r="178" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="178" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A178" s="8">
         <v>3.0514999999999999</v>
       </c>
@@ -8689,7 +8858,7 @@
         <v>-0.1837</v>
       </c>
     </row>
-    <row r="179" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="179" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A179" s="8">
         <v>3.6617999999999999</v>
       </c>
@@ -8745,7 +8914,7 @@
         <v>-9.1499999999999998E-2</v>
       </c>
     </row>
-    <row r="180" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="180" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A180" s="8">
         <v>4.2721</v>
       </c>
@@ -8801,7 +8970,7 @@
         <v>3.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="181" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="181" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A181" s="8">
         <v>4.8823999999999996</v>
       </c>
@@ -8857,7 +9026,7 @@
         <v>9.7199999999999995E-2</v>
       </c>
     </row>
-    <row r="182" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="182" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A182" s="8">
         <v>5.4927000000000001</v>
       </c>
@@ -8913,7 +9082,7 @@
         <v>0.18629999999999999</v>
       </c>
     </row>
-    <row r="183" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="183" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A183" s="8">
         <v>6.1029999999999998</v>
       </c>
@@ -8969,7 +9138,7 @@
         <v>0.26819999999999999</v>
       </c>
     </row>
-    <row r="184" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="184" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A184" s="8">
         <v>7.3235999999999999</v>
       </c>
@@ -9025,7 +9194,7 @@
         <v>0.40150000000000002</v>
       </c>
     </row>
-    <row r="185" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="185" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A185" s="8">
         <v>7.6287000000000003</v>
       </c>
@@ -9081,7 +9250,7 @@
         <v>0.42709999999999998</v>
       </c>
     </row>
-    <row r="186" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="186" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A186" s="8">
         <v>8.5442</v>
       </c>
@@ -9137,7 +9306,7 @@
         <v>0.49109999999999998</v>
       </c>
     </row>
-    <row r="187" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="187" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A187" s="8">
         <v>9.7647999999999993</v>
       </c>
@@ -9193,7 +9362,7 @@
         <v>0.56479999999999997</v>
       </c>
     </row>
-    <row r="188" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="188" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A188" s="8">
         <v>10.9854</v>
       </c>
@@ -9249,7 +9418,7 @@
         <v>0.62429999999999997</v>
       </c>
     </row>
-    <row r="189" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="189" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A189" s="8">
         <v>12.206</v>
       </c>
@@ -9305,7 +9474,7 @@
         <v>0.66900000000000004</v>
       </c>
     </row>
-    <row r="190" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="190" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A190" s="8">
         <v>13.426600000000001</v>
       </c>
@@ -9361,7 +9530,7 @@
         <v>0.6986</v>
       </c>
     </row>
-    <row r="191" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="191" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A191" s="8">
         <v>14.6472</v>
       </c>
@@ -9417,7 +9586,7 @@
         <v>0.71309999999999996</v>
       </c>
     </row>
-    <row r="192" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="192" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A192" s="8">
         <v>15.867800000000001</v>
       </c>
@@ -9473,7 +9642,7 @@
         <v>0.71250000000000002</v>
       </c>
     </row>
-    <row r="193" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="193" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A193" s="8">
         <v>17.0884</v>
       </c>
@@ -9529,7 +9698,7 @@
         <v>0.69750000000000001</v>
       </c>
     </row>
-    <row r="194" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="194" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A194" s="8">
         <v>18.309000000000001</v>
       </c>
@@ -9585,7 +9754,7 @@
         <v>0.66859999999999997</v>
       </c>
     </row>
-    <row r="195" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="195" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A195" s="8">
         <v>19.529599999999999</v>
       </c>
@@ -9641,7 +9810,7 @@
         <v>0.62649999999999995</v>
       </c>
     </row>
-    <row r="196" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="196" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A196" s="8">
         <v>20.7502</v>
       </c>
@@ -9697,7 +9866,7 @@
         <v>0.57889999999999997</v>
       </c>
     </row>
-    <row r="197" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="197" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A197" s="8">
         <v>21.970800000000001</v>
       </c>
@@ -9753,7 +9922,7 @@
         <v>0.52239999999999998</v>
       </c>
     </row>
-    <row r="198" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="198" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A198" s="8">
         <v>23.191400000000002</v>
       </c>
@@ -9809,7 +9978,7 @@
         <v>0.45590000000000003</v>
       </c>
     </row>
-    <row r="199" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="199" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A199" s="8">
         <v>24.411999999999999</v>
       </c>
@@ -9865,7 +10034,7 @@
         <v>0.38069999999999998</v>
       </c>
     </row>
-    <row r="200" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="200" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A200" s="8">
         <v>25.6326</v>
       </c>
@@ -9921,7 +10090,7 @@
         <v>0.29809999999999998</v>
       </c>
     </row>
-    <row r="201" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="201" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A201" s="8">
         <v>26.853200000000001</v>
       </c>
@@ -9977,7 +10146,7 @@
         <v>0.2092</v>
       </c>
     </row>
-    <row r="202" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="202" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A202" s="8">
         <v>28.073799999999999</v>
       </c>
@@ -10033,7 +10202,7 @@
         <v>0.115</v>
       </c>
     </row>
-    <row r="203" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="203" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A203" s="8">
         <v>29.2944</v>
       </c>
@@ -10089,7 +10258,7 @@
         <v>1.55E-2</v>
       </c>
     </row>
-    <row r="204" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="204" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A204" s="8">
         <v>29.904699999999998</v>
       </c>
@@ -10145,7 +10314,7 @@
         <v>-3.6900000000000002E-2</v>
       </c>
     </row>
-    <row r="205" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="205" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A205" s="8">
         <v>30.515000000000001</v>
       </c>
@@ -10201,7 +10370,7 @@
         <v>-9.3299999999999994E-2</v>
       </c>
     </row>
-    <row r="209" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="209" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A209" s="1" t="s">
         <v>8</v>
       </c>
@@ -10224,7 +10393,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="211" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="211" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A211" s="1" t="s">
         <v>53</v>
       </c>
@@ -10289,7 +10458,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="212" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="212" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A212" s="8">
         <v>0</v>
       </c>
@@ -10354,7 +10523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="213" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A213" s="8">
         <v>7.6899999999999996E-2</v>
       </c>
@@ -10419,7 +10588,7 @@
         <v>-6.7900000000000002E-2</v>
       </c>
     </row>
-    <row r="214" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="214" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A214" s="8">
         <v>0.15390000000000001</v>
       </c>
@@ -10484,7 +10653,7 @@
         <v>-9.3200000000000005E-2</v>
       </c>
     </row>
-    <row r="215" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="215" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A215" s="8">
         <v>0.23080000000000001</v>
       </c>
@@ -10549,7 +10718,7 @@
         <v>-0.1113</v>
       </c>
     </row>
-    <row r="216" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="216" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A216" s="8">
         <v>0.30780000000000002</v>
       </c>
@@ -10614,7 +10783,7 @@
         <v>-0.12570000000000001</v>
       </c>
     </row>
-    <row r="217" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="217" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A217" s="8">
         <v>0.38469999999999999</v>
       </c>
@@ -10679,7 +10848,7 @@
         <v>-0.1376</v>
       </c>
     </row>
-    <row r="218" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="218" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A218" s="8">
         <v>0.4617</v>
       </c>
@@ -10744,7 +10913,7 @@
         <v>-0.14779999999999999</v>
       </c>
     </row>
-    <row r="219" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="219" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A219" s="8">
         <v>0.53859999999999997</v>
       </c>
@@ -10809,7 +10978,7 @@
         <v>-0.15659999999999999</v>
       </c>
     </row>
-    <row r="220" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="220" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A220" s="8">
         <v>0.61560000000000004</v>
       </c>
@@ -10874,7 +11043,7 @@
         <v>-0.16439999999999999</v>
       </c>
     </row>
-    <row r="221" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="221" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A221" s="8">
         <v>0.76949999999999996</v>
       </c>
@@ -10939,7 +11108,7 @@
         <v>-0.1774</v>
       </c>
     </row>
-    <row r="222" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="222" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A222" s="8">
         <v>0.9234</v>
       </c>
@@ -11004,7 +11173,7 @@
         <v>-0.18790000000000001</v>
       </c>
     </row>
-    <row r="223" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="223" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A223" s="8">
         <v>1.0772999999999999</v>
       </c>
@@ -11069,7 +11238,7 @@
         <v>-0.1963</v>
       </c>
     </row>
-    <row r="224" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="224" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A224" s="8">
         <v>1.2312000000000001</v>
       </c>
@@ -11134,7 +11303,7 @@
         <v>-0.20319999999999999</v>
       </c>
     </row>
-    <row r="225" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="225" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A225" s="8">
         <v>1.3851</v>
       </c>
@@ -11199,7 +11368,7 @@
         <v>-0.20880000000000001</v>
       </c>
     </row>
-    <row r="226" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="226" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A226" s="8">
         <v>1.5388999999999999</v>
       </c>
@@ -11264,7 +11433,7 @@
         <v>-0.21329999999999999</v>
       </c>
     </row>
-    <row r="227" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="227" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A227" s="8">
         <v>1.8467</v>
       </c>
@@ -11329,7 +11498,7 @@
         <v>-0.21970000000000001</v>
       </c>
     </row>
-    <row r="228" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="228" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A228" s="8">
         <v>2.1545000000000001</v>
       </c>
@@ -11394,7 +11563,7 @@
         <v>-0.22320000000000001</v>
       </c>
     </row>
-    <row r="229" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="229" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A229" s="8">
         <v>2.4622999999999999</v>
       </c>
@@ -11459,7 +11628,7 @@
         <v>-0.22450000000000001</v>
       </c>
     </row>
-    <row r="230" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="230" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A230" s="8">
         <v>2.7700999999999998</v>
       </c>
@@ -11524,7 +11693,7 @@
         <v>-0.22409999999999999</v>
       </c>
     </row>
-    <row r="231" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="231" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A231" s="8">
         <v>3.0779000000000001</v>
       </c>
@@ -11589,7 +11758,7 @@
         <v>-0.2223</v>
       </c>
     </row>
-    <row r="232" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="232" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A232" s="8">
         <v>3.6934999999999998</v>
       </c>
@@ -11654,7 +11823,7 @@
         <v>-0.2155</v>
       </c>
     </row>
-    <row r="233" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="233" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A233" s="8">
         <v>4.3090000000000002</v>
       </c>
@@ -11719,7 +11888,7 @@
         <v>-0.2059</v>
       </c>
     </row>
-    <row r="234" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="234" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A234" s="8">
         <v>4.9245999999999999</v>
       </c>
@@ -11784,7 +11953,7 @@
         <v>-0.19439999999999999</v>
       </c>
     </row>
-    <row r="235" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="235" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A235" s="8">
         <v>5.5401999999999996</v>
       </c>
@@ -11849,7 +12018,7 @@
         <v>-0.18190000000000001</v>
       </c>
     </row>
-    <row r="236" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="236" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A236" s="8">
         <v>6.1558000000000002</v>
       </c>
@@ -11914,7 +12083,7 @@
         <v>-0.16919999999999999</v>
       </c>
     </row>
-    <row r="237" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="237" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A237" s="8">
         <v>7.3868999999999998</v>
       </c>
@@ -11979,7 +12148,7 @@
         <v>-0.1452</v>
       </c>
     </row>
-    <row r="238" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="238" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A238" s="8">
         <v>7.6947000000000001</v>
       </c>
@@ -12044,7 +12213,7 @@
         <v>-0.13980000000000001</v>
       </c>
     </row>
-    <row r="239" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="239" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A239" s="8">
         <v>8.6181000000000001</v>
       </c>
@@ -12109,7 +12278,7 @@
         <v>-0.12620000000000001</v>
       </c>
     </row>
-    <row r="240" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="240" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A240" s="8">
         <v>9.8491999999999997</v>
       </c>
@@ -12174,7 +12343,7 @@
         <v>-0.1086</v>
       </c>
     </row>
-    <row r="241" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="241" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A241" s="8">
         <v>11.080399999999999</v>
       </c>
@@ -12239,7 +12408,7 @@
         <v>-9.2399999999999996E-2</v>
       </c>
     </row>
-    <row r="242" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="242" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A242" s="8">
         <v>12.3116</v>
       </c>
@@ -12304,7 +12473,7 @@
         <v>-7.8299999999999995E-2</v>
       </c>
     </row>
-    <row r="243" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="243" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A243" s="8">
         <v>13.5427</v>
       </c>
@@ -12369,7 +12538,7 @@
         <v>-6.6600000000000006E-2</v>
       </c>
     </row>
-    <row r="244" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="244" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A244" s="8">
         <v>14.773899999999999</v>
       </c>
@@ -12434,7 +12603,7 @@
         <v>-5.74E-2</v>
       </c>
     </row>
-    <row r="245" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="245" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A245" s="8">
         <v>16.004999999999999</v>
       </c>
@@ -12499,7 +12668,7 @@
         <v>-5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="246" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="246" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A246" s="8">
         <v>17.2362</v>
       </c>
@@ -12564,7 +12733,7 @@
         <v>-4.6899999999999997E-2</v>
       </c>
     </row>
-    <row r="247" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="247" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A247" s="8">
         <v>18.467300000000002</v>
       </c>
@@ -12629,7 +12798,7 @@
         <v>-4.53E-2</v>
       </c>
     </row>
-    <row r="248" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="248" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A248" s="8">
         <v>19.698499999999999</v>
       </c>
@@ -12694,7 +12863,7 @@
         <v>-4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="249" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="249" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A249" s="8">
         <v>20.9297</v>
       </c>
@@ -12759,7 +12928,7 @@
         <v>-4.5499999999999999E-2</v>
       </c>
     </row>
-    <row r="250" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="250" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A250" s="8">
         <v>22.160799999999998</v>
       </c>
@@ -12824,7 +12993,7 @@
         <v>-4.5400000000000003E-2</v>
       </c>
     </row>
-    <row r="251" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="251" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A251" s="8">
         <v>23.391999999999999</v>
       </c>
@@ -12889,7 +13058,7 @@
         <v>-4.6300000000000001E-2</v>
       </c>
     </row>
-    <row r="252" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="252" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A252" s="8">
         <v>24.623100000000001</v>
       </c>
@@ -12954,7 +13123,7 @@
         <v>-4.7699999999999999E-2</v>
       </c>
     </row>
-    <row r="253" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="253" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A253" s="8">
         <v>25.854299999999999</v>
       </c>
@@ -13019,7 +13188,7 @@
         <v>-4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="254" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="254" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A254" s="8">
         <v>27.0854</v>
       </c>
@@ -13084,7 +13253,7 @@
         <v>-4.99E-2</v>
       </c>
     </row>
-    <row r="255" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="255" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A255" s="8">
         <v>28.316600000000001</v>
       </c>
@@ -13149,7 +13318,7 @@
         <v>-0.05</v>
       </c>
     </row>
-    <row r="256" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="256" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A256" s="8">
         <v>29.547699999999999</v>
       </c>
@@ -13214,7 +13383,7 @@
         <v>-4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="257" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="257" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A257" s="8">
         <v>30.1633</v>
       </c>
@@ -13279,7 +13448,7 @@
         <v>-4.9500000000000002E-2</v>
       </c>
     </row>
-    <row r="258" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="258" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A258" s="8">
         <v>30.7789</v>
       </c>
@@ -13344,7 +13513,7 @@
         <v>-5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="261" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="261" spans="1:27" x14ac:dyDescent="0.3">
       <c r="U261" s="8"/>
       <c r="V261" s="8"/>
       <c r="W261" s="8"/>
@@ -13352,7 +13521,7 @@
       <c r="Z261" s="8"/>
       <c r="AA261" s="8"/>
     </row>
-    <row r="262" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="262" spans="1:27" x14ac:dyDescent="0.3">
       <c r="U262" s="8"/>
       <c r="V262" s="8"/>
       <c r="W262" s="8"/>
@@ -13360,7 +13529,7 @@
       <c r="Z262" s="8"/>
       <c r="AA262" s="8"/>
     </row>
-    <row r="263" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="263" spans="1:27" x14ac:dyDescent="0.3">
       <c r="U263" s="8"/>
       <c r="V263" s="8"/>
       <c r="W263" s="8"/>
@@ -13368,7 +13537,7 @@
       <c r="Z263" s="8"/>
       <c r="AA263" s="8"/>
     </row>
-    <row r="264" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="264" spans="1:27" x14ac:dyDescent="0.3">
       <c r="U264" s="8"/>
       <c r="V264" s="8"/>
       <c r="W264" s="8"/>
@@ -13376,7 +13545,7 @@
       <c r="Z264" s="8"/>
       <c r="AA264" s="8"/>
     </row>
-    <row r="265" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="265" spans="1:27" x14ac:dyDescent="0.3">
       <c r="U265" s="8"/>
       <c r="V265" s="8"/>
       <c r="W265" s="8"/>
@@ -13384,7 +13553,7 @@
       <c r="Z265" s="8"/>
       <c r="AA265" s="8"/>
     </row>
-    <row r="266" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="266" spans="1:27" x14ac:dyDescent="0.3">
       <c r="U266" s="8"/>
       <c r="V266" s="8"/>
       <c r="W266" s="8"/>
@@ -13392,7 +13561,7 @@
       <c r="Z266" s="8"/>
       <c r="AA266" s="8"/>
     </row>
-    <row r="267" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="267" spans="1:27" x14ac:dyDescent="0.3">
       <c r="U267" s="8"/>
       <c r="V267" s="8"/>
       <c r="W267" s="8"/>
@@ -13400,7 +13569,7 @@
       <c r="Z267" s="8"/>
       <c r="AA267" s="8"/>
     </row>
-    <row r="268" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="268" spans="1:27" x14ac:dyDescent="0.3">
       <c r="U268" s="8"/>
       <c r="V268" s="8"/>
       <c r="W268" s="8"/>
@@ -13408,7 +13577,7 @@
       <c r="Z268" s="8"/>
       <c r="AA268" s="8"/>
     </row>
-    <row r="269" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="269" spans="1:27" x14ac:dyDescent="0.3">
       <c r="U269" s="8"/>
       <c r="V269" s="8"/>
       <c r="W269" s="8"/>
@@ -13416,7 +13585,7 @@
       <c r="Z269" s="8"/>
       <c r="AA269" s="8"/>
     </row>
-    <row r="270" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="270" spans="1:27" x14ac:dyDescent="0.3">
       <c r="U270" s="8"/>
       <c r="V270" s="8"/>
       <c r="W270" s="8"/>
@@ -13424,7 +13593,7 @@
       <c r="Z270" s="8"/>
       <c r="AA270" s="8"/>
     </row>
-    <row r="271" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="271" spans="1:27" x14ac:dyDescent="0.3">
       <c r="U271" s="8"/>
       <c r="V271" s="8"/>
       <c r="W271" s="8"/>
@@ -13432,7 +13601,7 @@
       <c r="Z271" s="8"/>
       <c r="AA271" s="8"/>
     </row>
-    <row r="272" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="272" spans="1:27" x14ac:dyDescent="0.3">
       <c r="U272" s="8"/>
       <c r="V272" s="8"/>
       <c r="W272" s="8"/>
@@ -13440,7 +13609,7 @@
       <c r="Z272" s="8"/>
       <c r="AA272" s="8"/>
     </row>
-    <row r="273" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="273" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U273" s="8"/>
       <c r="V273" s="8"/>
       <c r="W273" s="8"/>
@@ -13448,7 +13617,7 @@
       <c r="Z273" s="8"/>
       <c r="AA273" s="8"/>
     </row>
-    <row r="274" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="274" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U274" s="8"/>
       <c r="V274" s="8"/>
       <c r="W274" s="8"/>
@@ -13456,7 +13625,7 @@
       <c r="Z274" s="8"/>
       <c r="AA274" s="8"/>
     </row>
-    <row r="275" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="275" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U275" s="8"/>
       <c r="V275" s="8"/>
       <c r="W275" s="8"/>
@@ -13464,7 +13633,7 @@
       <c r="Z275" s="8"/>
       <c r="AA275" s="8"/>
     </row>
-    <row r="276" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="276" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U276" s="8"/>
       <c r="V276" s="8"/>
       <c r="W276" s="8"/>
@@ -13472,7 +13641,7 @@
       <c r="Z276" s="8"/>
       <c r="AA276" s="8"/>
     </row>
-    <row r="277" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="277" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U277" s="8"/>
       <c r="V277" s="8"/>
       <c r="W277" s="8"/>
@@ -13480,7 +13649,7 @@
       <c r="Z277" s="8"/>
       <c r="AA277" s="8"/>
     </row>
-    <row r="278" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="278" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U278" s="8"/>
       <c r="V278" s="8"/>
       <c r="W278" s="8"/>
@@ -13488,7 +13657,7 @@
       <c r="Z278" s="8"/>
       <c r="AA278" s="8"/>
     </row>
-    <row r="279" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="279" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U279" s="8"/>
       <c r="V279" s="8"/>
       <c r="W279" s="8"/>
@@ -13496,7 +13665,7 @@
       <c r="Z279" s="8"/>
       <c r="AA279" s="8"/>
     </row>
-    <row r="280" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="280" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U280" s="8"/>
       <c r="V280" s="8"/>
       <c r="W280" s="8"/>
@@ -13504,7 +13673,7 @@
       <c r="Z280" s="8"/>
       <c r="AA280" s="8"/>
     </row>
-    <row r="281" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="281" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U281" s="8"/>
       <c r="V281" s="8"/>
       <c r="W281" s="8"/>
@@ -13512,7 +13681,7 @@
       <c r="Z281" s="8"/>
       <c r="AA281" s="8"/>
     </row>
-    <row r="282" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="282" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U282" s="8"/>
       <c r="V282" s="8"/>
       <c r="W282" s="8"/>
@@ -13520,7 +13689,7 @@
       <c r="Z282" s="8"/>
       <c r="AA282" s="8"/>
     </row>
-    <row r="283" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="283" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U283" s="8"/>
       <c r="V283" s="8"/>
       <c r="W283" s="8"/>
@@ -13528,7 +13697,7 @@
       <c r="Z283" s="8"/>
       <c r="AA283" s="8"/>
     </row>
-    <row r="284" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="284" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U284" s="8"/>
       <c r="V284" s="8"/>
       <c r="W284" s="8"/>
@@ -13536,7 +13705,7 @@
       <c r="Z284" s="8"/>
       <c r="AA284" s="8"/>
     </row>
-    <row r="285" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="285" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U285" s="8"/>
       <c r="V285" s="8"/>
       <c r="W285" s="8"/>
@@ -13544,7 +13713,7 @@
       <c r="Z285" s="8"/>
       <c r="AA285" s="8"/>
     </row>
-    <row r="286" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="286" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U286" s="8"/>
       <c r="V286" s="8"/>
       <c r="W286" s="8"/>
@@ -13552,7 +13721,7 @@
       <c r="Z286" s="8"/>
       <c r="AA286" s="8"/>
     </row>
-    <row r="287" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="287" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U287" s="8"/>
       <c r="V287" s="8"/>
       <c r="W287" s="8"/>
@@ -13560,7 +13729,7 @@
       <c r="Z287" s="8"/>
       <c r="AA287" s="8"/>
     </row>
-    <row r="288" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="288" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U288" s="8"/>
       <c r="V288" s="8"/>
       <c r="W288" s="8"/>
@@ -13568,7 +13737,7 @@
       <c r="Z288" s="8"/>
       <c r="AA288" s="8"/>
     </row>
-    <row r="289" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="289" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U289" s="8"/>
       <c r="V289" s="8"/>
       <c r="W289" s="8"/>
@@ -13576,7 +13745,7 @@
       <c r="Z289" s="8"/>
       <c r="AA289" s="8"/>
     </row>
-    <row r="290" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="290" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U290" s="8"/>
       <c r="V290" s="8"/>
       <c r="W290" s="8"/>
@@ -13584,7 +13753,7 @@
       <c r="Z290" s="8"/>
       <c r="AA290" s="8"/>
     </row>
-    <row r="291" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="291" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U291" s="8"/>
       <c r="V291" s="8"/>
       <c r="W291" s="8"/>
@@ -13592,7 +13761,7 @@
       <c r="Z291" s="8"/>
       <c r="AA291" s="8"/>
     </row>
-    <row r="292" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="292" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U292" s="8"/>
       <c r="V292" s="8"/>
       <c r="W292" s="8"/>
@@ -13600,7 +13769,7 @@
       <c r="Z292" s="8"/>
       <c r="AA292" s="8"/>
     </row>
-    <row r="293" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="293" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U293" s="8"/>
       <c r="V293" s="8"/>
       <c r="W293" s="8"/>
@@ -13608,7 +13777,7 @@
       <c r="Z293" s="8"/>
       <c r="AA293" s="8"/>
     </row>
-    <row r="294" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="294" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U294" s="8"/>
       <c r="V294" s="8"/>
       <c r="W294" s="8"/>
@@ -13616,7 +13785,7 @@
       <c r="Z294" s="8"/>
       <c r="AA294" s="8"/>
     </row>
-    <row r="295" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="295" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U295" s="8"/>
       <c r="V295" s="8"/>
       <c r="W295" s="8"/>
@@ -13624,7 +13793,7 @@
       <c r="Z295" s="8"/>
       <c r="AA295" s="8"/>
     </row>
-    <row r="296" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="296" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U296" s="8"/>
       <c r="V296" s="8"/>
       <c r="W296" s="8"/>
@@ -13632,7 +13801,7 @@
       <c r="Z296" s="8"/>
       <c r="AA296" s="8"/>
     </row>
-    <row r="297" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="297" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U297" s="8"/>
       <c r="V297" s="8"/>
       <c r="W297" s="8"/>
@@ -13640,7 +13809,7 @@
       <c r="Z297" s="8"/>
       <c r="AA297" s="8"/>
     </row>
-    <row r="298" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="298" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U298" s="8"/>
       <c r="V298" s="8"/>
       <c r="W298" s="8"/>
@@ -13648,7 +13817,7 @@
       <c r="Z298" s="8"/>
       <c r="AA298" s="8"/>
     </row>
-    <row r="299" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="299" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U299" s="8"/>
       <c r="V299" s="8"/>
       <c r="W299" s="8"/>
@@ -13656,7 +13825,7 @@
       <c r="Z299" s="8"/>
       <c r="AA299" s="8"/>
     </row>
-    <row r="300" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="300" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U300" s="8"/>
       <c r="V300" s="8"/>
       <c r="W300" s="8"/>
@@ -13664,7 +13833,7 @@
       <c r="Z300" s="8"/>
       <c r="AA300" s="8"/>
     </row>
-    <row r="301" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="301" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U301" s="8"/>
       <c r="V301" s="8"/>
       <c r="W301" s="8"/>
@@ -13672,7 +13841,7 @@
       <c r="Z301" s="8"/>
       <c r="AA301" s="8"/>
     </row>
-    <row r="302" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="302" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U302" s="8"/>
       <c r="V302" s="8"/>
       <c r="W302" s="8"/>
@@ -13680,7 +13849,7 @@
       <c r="Z302" s="8"/>
       <c r="AA302" s="8"/>
     </row>
-    <row r="303" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="303" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U303" s="8"/>
       <c r="V303" s="8"/>
       <c r="W303" s="8"/>
@@ -13688,7 +13857,7 @@
       <c r="Z303" s="8"/>
       <c r="AA303" s="8"/>
     </row>
-    <row r="304" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="304" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U304" s="8"/>
       <c r="V304" s="8"/>
       <c r="W304" s="8"/>
@@ -13696,7 +13865,7 @@
       <c r="Z304" s="8"/>
       <c r="AA304" s="8"/>
     </row>
-    <row r="305" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="305" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U305" s="8"/>
       <c r="V305" s="8"/>
       <c r="W305" s="8"/>
@@ -13704,7 +13873,7 @@
       <c r="Z305" s="8"/>
       <c r="AA305" s="8"/>
     </row>
-    <row r="306" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="306" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U306" s="8"/>
       <c r="V306" s="8"/>
       <c r="W306" s="8"/>
@@ -13712,7 +13881,7 @@
       <c r="Z306" s="8"/>
       <c r="AA306" s="8"/>
     </row>
-    <row r="307" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="307" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U307" s="8"/>
       <c r="V307" s="8"/>
       <c r="W307" s="8"/>
@@ -13720,82 +13889,82 @@
       <c r="Z307" s="8"/>
       <c r="AA307" s="8"/>
     </row>
-    <row r="308" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="308" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U308" s="8"/>
       <c r="V308" s="8"/>
       <c r="W308" s="8"/>
     </row>
-    <row r="309" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="309" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U309" s="8"/>
       <c r="V309" s="8"/>
       <c r="W309" s="8"/>
     </row>
-    <row r="310" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="310" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U310" s="8"/>
       <c r="V310" s="8"/>
       <c r="W310" s="8"/>
     </row>
-    <row r="311" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="311" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U311" s="8"/>
       <c r="V311" s="8"/>
       <c r="W311" s="8"/>
     </row>
-    <row r="312" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="312" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U312" s="8"/>
       <c r="V312" s="8"/>
       <c r="W312" s="8"/>
     </row>
-    <row r="313" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="313" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U313" s="8"/>
       <c r="V313" s="8"/>
       <c r="W313" s="8"/>
     </row>
-    <row r="314" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="314" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U314" s="8"/>
       <c r="V314" s="8"/>
       <c r="W314" s="8"/>
     </row>
-    <row r="315" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="315" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U315" s="8"/>
       <c r="V315" s="8"/>
       <c r="W315" s="8"/>
     </row>
-    <row r="316" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="316" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U316" s="8"/>
       <c r="V316" s="8"/>
       <c r="W316" s="8"/>
     </row>
-    <row r="317" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="317" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U317" s="8"/>
       <c r="V317" s="8"/>
       <c r="W317" s="8"/>
     </row>
-    <row r="318" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="318" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U318" s="8"/>
       <c r="V318" s="8"/>
       <c r="W318" s="8"/>
     </row>
-    <row r="319" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="319" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U319" s="8"/>
       <c r="V319" s="8"/>
       <c r="W319" s="8"/>
     </row>
-    <row r="320" spans="21:27" x14ac:dyDescent="0.4">
+    <row r="320" spans="21:27" x14ac:dyDescent="0.3">
       <c r="U320" s="8"/>
       <c r="V320" s="8"/>
       <c r="W320" s="8"/>
     </row>
-    <row r="321" spans="21:23" x14ac:dyDescent="0.4">
+    <row r="321" spans="21:23" x14ac:dyDescent="0.3">
       <c r="U321" s="8"/>
       <c r="V321" s="8"/>
       <c r="W321" s="8"/>
     </row>
-    <row r="322" spans="21:23" x14ac:dyDescent="0.4">
+    <row r="322" spans="21:23" x14ac:dyDescent="0.3">
       <c r="U322" s="8"/>
       <c r="V322" s="8"/>
       <c r="W322" s="8"/>
     </row>
-    <row r="323" spans="21:23" x14ac:dyDescent="0.4">
+    <row r="323" spans="21:23" x14ac:dyDescent="0.3">
       <c r="U323" s="8"/>
       <c r="V323" s="8"/>
       <c r="W323" s="8"/>

</xml_diff>